<commit_message>
Update Master Chart Data
</commit_message>
<xml_diff>
--- a/Master Chart Data.xlsx
+++ b/Master Chart Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherineravenwood/Documents/GitHub/Spotify-Five-Year-Analysis-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA3F77F-E0AD-5746-8019-2B21BEAABE07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8658B99F-4E11-F44C-A458-7C35296B201A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{BA16DD78-4E07-0B46-959B-144C800F05BB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{BA16DD78-4E07-0B46-959B-144C800F05BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Albums Playlists" sheetId="1" r:id="rId1"/>
@@ -2746,6 +2746,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2761,7 +2762,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3684,7 +3684,7 @@
       <c r="D28" t="s">
         <v>54</v>
       </c>
-      <c r="E28" s="13" t="b">
+      <c r="E28" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3701,7 +3701,7 @@
       <c r="D29" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="13" t="b">
+      <c r="E29" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3718,7 +3718,7 @@
       <c r="D30" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="13" t="b">
+      <c r="E30" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3735,7 +3735,7 @@
       <c r="D31" t="s">
         <v>59</v>
       </c>
-      <c r="E31" s="13" t="b">
+      <c r="E31" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3752,7 +3752,7 @@
       <c r="D32" t="s">
         <v>29</v>
       </c>
-      <c r="E32" s="13" t="b">
+      <c r="E32" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3769,7 +3769,7 @@
       <c r="D33" t="s">
         <v>62</v>
       </c>
-      <c r="E33" s="13" t="b">
+      <c r="E33" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3786,7 +3786,7 @@
       <c r="D34" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="13" t="b">
+      <c r="E34" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3803,7 +3803,7 @@
       <c r="D35" t="s">
         <v>65</v>
       </c>
-      <c r="E35" s="13" t="b">
+      <c r="E35" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3820,7 +3820,7 @@
       <c r="D36" t="s">
         <v>35</v>
       </c>
-      <c r="E36" s="13" t="b">
+      <c r="E36" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3837,7 +3837,7 @@
       <c r="D37" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="13" t="b">
+      <c r="E37" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3854,7 +3854,7 @@
       <c r="D38" t="s">
         <v>69</v>
       </c>
-      <c r="E38" s="13" t="b">
+      <c r="E38" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3871,7 +3871,7 @@
       <c r="D39" t="s">
         <v>71</v>
       </c>
-      <c r="E39" s="13" t="b">
+      <c r="E39" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3888,7 +3888,7 @@
       <c r="D40" t="s">
         <v>73</v>
       </c>
-      <c r="E40" s="13" t="b">
+      <c r="E40" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3905,7 +3905,7 @@
       <c r="D41" t="s">
         <v>75</v>
       </c>
-      <c r="E41" s="13" t="b">
+      <c r="E41" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3922,7 +3922,7 @@
       <c r="D42" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="13" t="b">
+      <c r="E42" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3939,7 +3939,7 @@
       <c r="D43" t="s">
         <v>24</v>
       </c>
-      <c r="E43" s="13" t="b">
+      <c r="E43" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3956,7 +3956,7 @@
       <c r="D44" t="s">
         <v>79</v>
       </c>
-      <c r="E44" s="13" t="b">
+      <c r="E44" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3973,7 +3973,7 @@
       <c r="D45" t="s">
         <v>41</v>
       </c>
-      <c r="E45" s="13" t="b">
+      <c r="E45" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3990,7 +3990,7 @@
       <c r="D46" t="s">
         <v>82</v>
       </c>
-      <c r="E46" s="13" t="b">
+      <c r="E46" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4007,7 +4007,7 @@
       <c r="D47" t="s">
         <v>84</v>
       </c>
-      <c r="E47" s="13" t="b">
+      <c r="E47" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4024,7 +4024,7 @@
       <c r="D48" t="s">
         <v>86</v>
       </c>
-      <c r="E48" s="13" t="b">
+      <c r="E48" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4041,7 +4041,7 @@
       <c r="D49" t="s">
         <v>84</v>
       </c>
-      <c r="E49" s="13" t="b">
+      <c r="E49" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4058,7 +4058,7 @@
       <c r="D50" t="s">
         <v>43</v>
       </c>
-      <c r="E50" s="13" t="b">
+      <c r="E50" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4075,7 +4075,7 @@
       <c r="D51" t="s">
         <v>27</v>
       </c>
-      <c r="E51" s="13" t="b">
+      <c r="E51" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4092,7 +4092,7 @@
       <c r="D52" t="s">
         <v>91</v>
       </c>
-      <c r="E52" s="13" t="b">
+      <c r="E52" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4109,7 +4109,7 @@
       <c r="D53" t="s">
         <v>93</v>
       </c>
-      <c r="E53" s="13" t="b">
+      <c r="E53" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4126,7 +4126,7 @@
       <c r="D54" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="13" t="b">
+      <c r="E54" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4143,7 +4143,7 @@
       <c r="D55" t="s">
         <v>12</v>
       </c>
-      <c r="E55" s="13" t="b">
+      <c r="E55" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4160,7 +4160,7 @@
       <c r="D56" t="s">
         <v>98</v>
       </c>
-      <c r="E56" s="13" t="b">
+      <c r="E56" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4177,7 +4177,7 @@
       <c r="D57" t="s">
         <v>100</v>
       </c>
-      <c r="E57" s="13" t="b">
+      <c r="E57" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4194,7 +4194,7 @@
       <c r="D58" t="s">
         <v>62</v>
       </c>
-      <c r="E58" s="13" t="b">
+      <c r="E58" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4211,7 +4211,7 @@
       <c r="D59" t="s">
         <v>59</v>
       </c>
-      <c r="E59" s="13" t="b">
+      <c r="E59" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4228,7 +4228,7 @@
       <c r="D60" t="s">
         <v>104</v>
       </c>
-      <c r="E60" s="13" t="b">
+      <c r="E60" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4245,7 +4245,7 @@
       <c r="D61" t="s">
         <v>106</v>
       </c>
-      <c r="E61" s="13" t="b">
+      <c r="E61" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4262,7 +4262,7 @@
       <c r="D62" t="s">
         <v>10</v>
       </c>
-      <c r="E62" s="13" t="b">
+      <c r="E62" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4279,7 +4279,7 @@
       <c r="D63" t="s">
         <v>56</v>
       </c>
-      <c r="E63" s="13" t="b">
+      <c r="E63" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4296,7 +4296,7 @@
       <c r="D64" t="s">
         <v>110</v>
       </c>
-      <c r="E64" s="13" t="b">
+      <c r="E64" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4313,7 +4313,7 @@
       <c r="D65" t="s">
         <v>112</v>
       </c>
-      <c r="E65" s="13" t="b">
+      <c r="E65" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4330,7 +4330,7 @@
       <c r="D66" t="s">
         <v>114</v>
       </c>
-      <c r="E66" s="13" t="b">
+      <c r="E66" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4347,7 +4347,7 @@
       <c r="D67" t="s">
         <v>116</v>
       </c>
-      <c r="E67" s="13" t="b">
+      <c r="E67" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4364,7 +4364,7 @@
       <c r="D68" t="s">
         <v>27</v>
       </c>
-      <c r="E68" s="13" t="b">
+      <c r="E68" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4381,7 +4381,7 @@
       <c r="D69" t="s">
         <v>119</v>
       </c>
-      <c r="E69" s="13" t="b">
+      <c r="E69" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4398,7 +4398,7 @@
       <c r="D70" t="s">
         <v>121</v>
       </c>
-      <c r="E70" s="13" t="b">
+      <c r="E70" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4415,7 +4415,7 @@
       <c r="D71" t="s">
         <v>54</v>
       </c>
-      <c r="E71" s="13" t="b">
+      <c r="E71" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4432,7 +4432,7 @@
       <c r="D72" t="s">
         <v>124</v>
       </c>
-      <c r="E72" s="13" t="b">
+      <c r="E72" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4449,7 +4449,7 @@
       <c r="D73" t="s">
         <v>126</v>
       </c>
-      <c r="E73" s="13" t="b">
+      <c r="E73" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4466,7 +4466,7 @@
       <c r="D74" t="s">
         <v>128</v>
       </c>
-      <c r="E74" s="13" t="b">
+      <c r="E74" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4483,7 +4483,7 @@
       <c r="D75" t="s">
         <v>130</v>
       </c>
-      <c r="E75" s="13" t="b">
+      <c r="E75" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4500,7 +4500,7 @@
       <c r="D76" t="s">
         <v>132</v>
       </c>
-      <c r="E76" s="13" t="b">
+      <c r="E76" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4517,7 +4517,7 @@
       <c r="D77" t="s">
         <v>133</v>
       </c>
-      <c r="E77" s="13" t="b">
+      <c r="E77" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4534,7 +4534,7 @@
       <c r="D78" t="s">
         <v>39</v>
       </c>
-      <c r="E78" s="13" t="b">
+      <c r="E78" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4551,7 +4551,7 @@
       <c r="D79" t="s">
         <v>12</v>
       </c>
-      <c r="E79" s="13" t="b">
+      <c r="E79" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4568,7 +4568,7 @@
       <c r="D80" t="s">
         <v>137</v>
       </c>
-      <c r="E80" s="13" t="b">
+      <c r="E80" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4585,7 +4585,7 @@
       <c r="D81" t="s">
         <v>100</v>
       </c>
-      <c r="E81" s="13" t="b">
+      <c r="E81" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4602,7 +4602,7 @@
       <c r="D82" t="s">
         <v>139</v>
       </c>
-      <c r="E82" s="13" t="b">
+      <c r="E82" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4619,7 +4619,7 @@
       <c r="D83" t="s">
         <v>95</v>
       </c>
-      <c r="E83" s="13" t="b">
+      <c r="E83" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4636,7 +4636,7 @@
       <c r="D84" t="s">
         <v>142</v>
       </c>
-      <c r="E84" s="13" t="b">
+      <c r="E84" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4653,7 +4653,7 @@
       <c r="D85" t="s">
         <v>143</v>
       </c>
-      <c r="E85" s="13" t="b">
+      <c r="E85" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4670,7 +4670,7 @@
       <c r="D86" t="s">
         <v>145</v>
       </c>
-      <c r="E86" s="13" t="b">
+      <c r="E86" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4687,7 +4687,7 @@
       <c r="D87" t="s">
         <v>147</v>
       </c>
-      <c r="E87" s="13" t="b">
+      <c r="E87" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4704,7 +4704,7 @@
       <c r="D88" t="s">
         <v>149</v>
       </c>
-      <c r="E88" s="13" t="b">
+      <c r="E88" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4721,7 +4721,7 @@
       <c r="D89" t="s">
         <v>10</v>
       </c>
-      <c r="E89" s="13" t="b">
+      <c r="E89" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4738,7 +4738,7 @@
       <c r="D90" t="s">
         <v>151</v>
       </c>
-      <c r="E90" s="13" t="b">
+      <c r="E90" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4755,7 +4755,7 @@
       <c r="D91" t="s">
         <v>153</v>
       </c>
-      <c r="E91" s="13" t="b">
+      <c r="E91" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4772,7 +4772,7 @@
       <c r="D92" t="s">
         <v>155</v>
       </c>
-      <c r="E92" s="13" t="b">
+      <c r="E92" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4789,7 +4789,7 @@
       <c r="D93" t="s">
         <v>18</v>
       </c>
-      <c r="E93" s="13" t="b">
+      <c r="E93" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4806,7 +4806,7 @@
       <c r="D94" t="s">
         <v>158</v>
       </c>
-      <c r="E94" s="13" t="b">
+      <c r="E94" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4823,7 +4823,7 @@
       <c r="D95" t="s">
         <v>160</v>
       </c>
-      <c r="E95" s="13" t="b">
+      <c r="E95" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4840,7 +4840,7 @@
       <c r="D96" t="s">
         <v>162</v>
       </c>
-      <c r="E96" s="13" t="b">
+      <c r="E96" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4857,7 +4857,7 @@
       <c r="D97" t="s">
         <v>143</v>
       </c>
-      <c r="E97" s="13" t="b">
+      <c r="E97" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4874,7 +4874,7 @@
       <c r="D98" t="s">
         <v>165</v>
       </c>
-      <c r="E98" s="13" t="b">
+      <c r="E98" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4891,7 +4891,7 @@
       <c r="D99" t="s">
         <v>167</v>
       </c>
-      <c r="E99" s="13" t="b">
+      <c r="E99" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4908,7 +4908,7 @@
       <c r="D100" t="s">
         <v>168</v>
       </c>
-      <c r="E100" s="13" t="b">
+      <c r="E100" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4925,7 +4925,7 @@
       <c r="D101" t="s">
         <v>170</v>
       </c>
-      <c r="E101" s="13" t="b">
+      <c r="E101" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4942,7 +4942,7 @@
       <c r="D102" t="s">
         <v>8</v>
       </c>
-      <c r="E102" s="13" t="b">
+      <c r="E102" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4959,7 +4959,7 @@
       <c r="D103" t="s">
         <v>173</v>
       </c>
-      <c r="E103" s="13" t="b">
+      <c r="E103" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4976,7 +4976,7 @@
       <c r="D104" t="s">
         <v>12</v>
       </c>
-      <c r="E104" s="13" t="b">
+      <c r="E104" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4993,7 +4993,7 @@
       <c r="D105" t="s">
         <v>176</v>
       </c>
-      <c r="E105" s="13" t="b">
+      <c r="E105" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5010,7 +5010,7 @@
       <c r="D106" t="s">
         <v>177</v>
       </c>
-      <c r="E106" s="13" t="b">
+      <c r="E106" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5027,7 +5027,7 @@
       <c r="D107" t="s">
         <v>179</v>
       </c>
-      <c r="E107" s="13" t="b">
+      <c r="E107" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5044,7 +5044,7 @@
       <c r="D108" t="s">
         <v>181</v>
       </c>
-      <c r="E108" s="13" t="b">
+      <c r="E108" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5061,7 +5061,7 @@
       <c r="D109" t="s">
         <v>183</v>
       </c>
-      <c r="E109" s="13" t="b">
+      <c r="E109" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5078,7 +5078,7 @@
       <c r="D110" t="s">
         <v>145</v>
       </c>
-      <c r="E110" s="13" t="b">
+      <c r="E110" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5095,7 +5095,7 @@
       <c r="D111" t="s">
         <v>186</v>
       </c>
-      <c r="E111" s="13" t="b">
+      <c r="E111" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5112,7 +5112,7 @@
       <c r="D112" t="s">
         <v>188</v>
       </c>
-      <c r="E112" s="13" t="b">
+      <c r="E112" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5129,7 +5129,7 @@
       <c r="D113" t="s">
         <v>190</v>
       </c>
-      <c r="E113" s="13" t="b">
+      <c r="E113" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5146,7 +5146,7 @@
       <c r="D114" t="s">
         <v>75</v>
       </c>
-      <c r="E114" s="13" t="b">
+      <c r="E114" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5163,7 +5163,7 @@
       <c r="D115" t="s">
         <v>193</v>
       </c>
-      <c r="E115" s="13" t="b">
+      <c r="E115" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5180,7 +5180,7 @@
       <c r="D116" t="s">
         <v>194</v>
       </c>
-      <c r="E116" s="13" t="b">
+      <c r="E116" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5197,7 +5197,7 @@
       <c r="D117" t="s">
         <v>59</v>
       </c>
-      <c r="E117" s="13" t="b">
+      <c r="E117" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5214,7 +5214,7 @@
       <c r="D118" t="s">
         <v>12</v>
       </c>
-      <c r="E118" s="13" t="b">
+      <c r="E118" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5231,7 +5231,7 @@
       <c r="D119" t="s">
         <v>198</v>
       </c>
-      <c r="E119" s="13" t="b">
+      <c r="E119" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5248,7 +5248,7 @@
       <c r="D120" t="s">
         <v>200</v>
       </c>
-      <c r="E120" s="13" t="b">
+      <c r="E120" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5265,7 +5265,7 @@
       <c r="D121" t="s">
         <v>202</v>
       </c>
-      <c r="E121" s="13" t="b">
+      <c r="E121" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5282,7 +5282,7 @@
       <c r="D122" t="s">
         <v>204</v>
       </c>
-      <c r="E122" s="13" t="b">
+      <c r="E122" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5299,7 +5299,7 @@
       <c r="D123" t="s">
         <v>206</v>
       </c>
-      <c r="E123" s="13" t="b">
+      <c r="E123" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5316,7 +5316,7 @@
       <c r="D124" t="s">
         <v>179</v>
       </c>
-      <c r="E124" s="13" t="b">
+      <c r="E124" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5333,7 +5333,7 @@
       <c r="D125" t="s">
         <v>112</v>
       </c>
-      <c r="E125" s="13" t="b">
+      <c r="E125" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5350,7 +5350,7 @@
       <c r="D126" t="s">
         <v>209</v>
       </c>
-      <c r="E126" s="13" t="b">
+      <c r="E126" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5367,7 +5367,7 @@
       <c r="D127" t="s">
         <v>211</v>
       </c>
-      <c r="E127" s="13" t="b">
+      <c r="E127" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5384,7 +5384,7 @@
       <c r="D128" t="s">
         <v>213</v>
       </c>
-      <c r="E128" s="13" t="b">
+      <c r="E128" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5401,7 +5401,7 @@
       <c r="D129" t="s">
         <v>82</v>
       </c>
-      <c r="E129" s="13" t="b">
+      <c r="E129" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5418,7 +5418,7 @@
       <c r="D130" t="s">
         <v>216</v>
       </c>
-      <c r="E130" s="13" t="b">
+      <c r="E130" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5435,7 +5435,7 @@
       <c r="D131" t="s">
         <v>73</v>
       </c>
-      <c r="E131" s="13" t="b">
+      <c r="E131" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5452,7 +5452,7 @@
       <c r="D132" t="s">
         <v>112</v>
       </c>
-      <c r="E132" s="13" t="b">
+      <c r="E132" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5469,7 +5469,7 @@
       <c r="D133" t="s">
         <v>220</v>
       </c>
-      <c r="E133" s="13" t="b">
+      <c r="E133" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5486,7 +5486,7 @@
       <c r="D134" t="s">
         <v>12</v>
       </c>
-      <c r="E134" s="13" t="b">
+      <c r="E134" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5503,7 +5503,7 @@
       <c r="D135" t="s">
         <v>188</v>
       </c>
-      <c r="E135" s="13" t="b">
+      <c r="E135" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5520,7 +5520,7 @@
       <c r="D136" t="s">
         <v>65</v>
       </c>
-      <c r="E136" s="13" t="b">
+      <c r="E136" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5537,7 +5537,7 @@
       <c r="D137" t="s">
         <v>224</v>
       </c>
-      <c r="E137" s="13" t="b">
+      <c r="E137" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5554,7 +5554,7 @@
       <c r="D138" t="s">
         <v>33</v>
       </c>
-      <c r="E138" s="13" t="b">
+      <c r="E138" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5571,7 +5571,7 @@
       <c r="D139" t="s">
         <v>226</v>
       </c>
-      <c r="E139" s="13" t="b">
+      <c r="E139" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5588,7 +5588,7 @@
       <c r="D140" t="s">
         <v>228</v>
       </c>
-      <c r="E140" s="13" t="b">
+      <c r="E140" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5605,7 +5605,7 @@
       <c r="D141" t="s">
         <v>230</v>
       </c>
-      <c r="E141" s="13" t="b">
+      <c r="E141" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5622,7 +5622,7 @@
       <c r="D142" t="s">
         <v>35</v>
       </c>
-      <c r="E142" s="13" t="b">
+      <c r="E142" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5639,7 +5639,7 @@
       <c r="D143" t="s">
         <v>233</v>
       </c>
-      <c r="E143" s="13" t="b">
+      <c r="E143" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5656,7 +5656,7 @@
       <c r="D144" t="s">
         <v>12</v>
       </c>
-      <c r="E144" s="13" t="b">
+      <c r="E144" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5673,7 +5673,7 @@
       <c r="D145" t="s">
         <v>236</v>
       </c>
-      <c r="E145" s="13" t="b">
+      <c r="E145" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5690,7 +5690,7 @@
       <c r="D146" t="s">
         <v>170</v>
       </c>
-      <c r="E146" s="13" t="b">
+      <c r="E146" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5707,7 +5707,7 @@
       <c r="D147" t="s">
         <v>239</v>
       </c>
-      <c r="E147" s="13" t="b">
+      <c r="E147" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5724,7 +5724,7 @@
       <c r="D148" t="s">
         <v>241</v>
       </c>
-      <c r="E148" s="13" t="b">
+      <c r="E148" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5741,7 +5741,7 @@
       <c r="D149" t="s">
         <v>242</v>
       </c>
-      <c r="E149" s="13" t="b">
+      <c r="E149" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5758,7 +5758,7 @@
       <c r="D150" t="s">
         <v>244</v>
       </c>
-      <c r="E150" s="13" t="b">
+      <c r="E150" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5775,7 +5775,7 @@
       <c r="D151" t="s">
         <v>153</v>
       </c>
-      <c r="E151" s="13" t="b">
+      <c r="E151" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5792,7 +5792,7 @@
       <c r="D152" t="s">
         <v>247</v>
       </c>
-      <c r="E152" s="13" t="b">
+      <c r="E152" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5809,7 +5809,7 @@
       <c r="D153" t="s">
         <v>73</v>
       </c>
-      <c r="E153" s="13" t="b">
+      <c r="E153" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5826,7 +5826,7 @@
       <c r="D154" t="s">
         <v>250</v>
       </c>
-      <c r="E154" s="13" t="b">
+      <c r="E154" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5843,7 +5843,7 @@
       <c r="D155" t="s">
         <v>252</v>
       </c>
-      <c r="E155" s="13" t="b">
+      <c r="E155" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5860,7 +5860,7 @@
       <c r="D156" t="s">
         <v>254</v>
       </c>
-      <c r="E156" s="13" t="b">
+      <c r="E156" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5877,7 +5877,7 @@
       <c r="D157" t="s">
         <v>170</v>
       </c>
-      <c r="E157" s="13" t="b">
+      <c r="E157" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5894,7 +5894,7 @@
       <c r="D158" t="s">
         <v>43</v>
       </c>
-      <c r="E158" s="13" t="b">
+      <c r="E158" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5911,7 +5911,7 @@
       <c r="D159" t="s">
         <v>258</v>
       </c>
-      <c r="E159" s="13" t="b">
+      <c r="E159" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5928,7 +5928,7 @@
       <c r="D160" t="s">
         <v>260</v>
       </c>
-      <c r="E160" s="13" t="b">
+      <c r="E160" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5945,7 +5945,7 @@
       <c r="D161" t="s">
         <v>130</v>
       </c>
-      <c r="E161" s="13" t="b">
+      <c r="E161" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5962,7 +5962,7 @@
       <c r="D162" t="s">
         <v>262</v>
       </c>
-      <c r="E162" s="13" t="b">
+      <c r="E162" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5979,7 +5979,7 @@
       <c r="D163" t="s">
         <v>29</v>
       </c>
-      <c r="E163" s="13" t="b">
+      <c r="E163" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5996,7 +5996,7 @@
       <c r="D164" t="s">
         <v>128</v>
       </c>
-      <c r="E164" s="13" t="b">
+      <c r="E164" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6013,7 +6013,7 @@
       <c r="D165" t="s">
         <v>266</v>
       </c>
-      <c r="E165" s="13" t="b">
+      <c r="E165" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6030,7 +6030,7 @@
       <c r="D166" t="s">
         <v>268</v>
       </c>
-      <c r="E166" s="13" t="b">
+      <c r="E166" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6047,7 +6047,7 @@
       <c r="D167" t="s">
         <v>270</v>
       </c>
-      <c r="E167" s="13" t="b">
+      <c r="E167" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6064,7 +6064,7 @@
       <c r="D168" t="s">
         <v>8</v>
       </c>
-      <c r="E168" s="13" t="b">
+      <c r="E168" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6081,7 +6081,7 @@
       <c r="D169" t="s">
         <v>93</v>
       </c>
-      <c r="E169" s="13" t="b">
+      <c r="E169" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6098,7 +6098,7 @@
       <c r="D170" t="s">
         <v>52</v>
       </c>
-      <c r="E170" s="13" t="b">
+      <c r="E170" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6115,7 +6115,7 @@
       <c r="D171" t="s">
         <v>10</v>
       </c>
-      <c r="E171" s="13" t="b">
+      <c r="E171" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6132,7 +6132,7 @@
       <c r="D172" t="s">
         <v>276</v>
       </c>
-      <c r="E172" s="13" t="b">
+      <c r="E172" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6149,7 +6149,7 @@
       <c r="D173" t="s">
         <v>278</v>
       </c>
-      <c r="E173" s="13" t="b">
+      <c r="E173" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6166,7 +6166,7 @@
       <c r="D174" t="s">
         <v>280</v>
       </c>
-      <c r="E174" s="13" t="b">
+      <c r="E174" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6183,7 +6183,7 @@
       <c r="D175" t="s">
         <v>119</v>
       </c>
-      <c r="E175" s="13" t="b">
+      <c r="E175" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6200,7 +6200,7 @@
       <c r="D176" t="s">
         <v>283</v>
       </c>
-      <c r="E176" s="13" t="b">
+      <c r="E176" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6217,7 +6217,7 @@
       <c r="D177" t="s">
         <v>285</v>
       </c>
-      <c r="E177" s="13" t="b">
+      <c r="E177" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6234,7 +6234,7 @@
       <c r="D178" t="s">
         <v>287</v>
       </c>
-      <c r="E178" s="13" t="b">
+      <c r="E178" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6251,7 +6251,7 @@
       <c r="D179" t="s">
         <v>289</v>
       </c>
-      <c r="E179" s="13" t="b">
+      <c r="E179" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6268,7 +6268,7 @@
       <c r="D180" t="s">
         <v>290</v>
       </c>
-      <c r="E180" s="13" t="b">
+      <c r="E180" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6285,7 +6285,7 @@
       <c r="D181" t="s">
         <v>292</v>
       </c>
-      <c r="E181" s="13" t="b">
+      <c r="E181" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6302,7 +6302,7 @@
       <c r="D182" t="s">
         <v>294</v>
       </c>
-      <c r="E182" s="13" t="b">
+      <c r="E182" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6319,7 +6319,7 @@
       <c r="D183" t="s">
         <v>151</v>
       </c>
-      <c r="E183" s="13" t="b">
+      <c r="E183" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6336,7 +6336,7 @@
       <c r="D184" t="s">
         <v>296</v>
       </c>
-      <c r="E184" s="13" t="b">
+      <c r="E184" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6353,7 +6353,7 @@
       <c r="D185" t="s">
         <v>298</v>
       </c>
-      <c r="E185" s="13" t="b">
+      <c r="E185" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6370,7 +6370,7 @@
       <c r="D186" t="s">
         <v>300</v>
       </c>
-      <c r="E186" s="13" t="b">
+      <c r="E186" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6387,7 +6387,7 @@
       <c r="D187" t="s">
         <v>302</v>
       </c>
-      <c r="E187" s="13" t="b">
+      <c r="E187" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6404,7 +6404,7 @@
       <c r="D188" t="s">
         <v>304</v>
       </c>
-      <c r="E188" s="13" t="b">
+      <c r="E188" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6421,7 +6421,7 @@
       <c r="D189" t="s">
         <v>306</v>
       </c>
-      <c r="E189" s="13" t="b">
+      <c r="E189" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6438,7 +6438,7 @@
       <c r="D190" t="s">
         <v>308</v>
       </c>
-      <c r="E190" s="13" t="b">
+      <c r="E190" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6455,7 +6455,7 @@
       <c r="D191" t="s">
         <v>310</v>
       </c>
-      <c r="E191" s="13" t="b">
+      <c r="E191" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6472,7 +6472,7 @@
       <c r="D192" t="s">
         <v>306</v>
       </c>
-      <c r="E192" s="13" t="b">
+      <c r="E192" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6489,7 +6489,7 @@
       <c r="D193" t="s">
         <v>313</v>
       </c>
-      <c r="E193" s="13" t="b">
+      <c r="E193" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6506,7 +6506,7 @@
       <c r="D194" t="s">
         <v>254</v>
       </c>
-      <c r="E194" s="13" t="b">
+      <c r="E194" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6523,7 +6523,7 @@
       <c r="D195" t="s">
         <v>316</v>
       </c>
-      <c r="E195" s="13" t="b">
+      <c r="E195" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6540,7 +6540,7 @@
       <c r="D196" t="s">
         <v>318</v>
       </c>
-      <c r="E196" s="13" t="b">
+      <c r="E196" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6557,7 +6557,7 @@
       <c r="D197" t="s">
         <v>320</v>
       </c>
-      <c r="E197" s="13" t="b">
+      <c r="E197" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6574,7 +6574,7 @@
       <c r="D198" t="s">
         <v>322</v>
       </c>
-      <c r="E198" s="13" t="b">
+      <c r="E198" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6591,7 +6591,7 @@
       <c r="D199" t="s">
         <v>323</v>
       </c>
-      <c r="E199" s="13" t="b">
+      <c r="E199" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6608,7 +6608,7 @@
       <c r="D200" t="s">
         <v>325</v>
       </c>
-      <c r="E200" s="13" t="b">
+      <c r="E200" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6625,7 +6625,7 @@
       <c r="D201" t="s">
         <v>327</v>
       </c>
-      <c r="E201" s="13" t="b">
+      <c r="E201" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7428,7 +7428,7 @@
       <c r="D45" t="s">
         <v>79</v>
       </c>
-      <c r="E45" s="13" t="b">
+      <c r="E45" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7445,7 +7445,7 @@
       <c r="D46" t="s">
         <v>27</v>
       </c>
-      <c r="E46" s="13" t="b">
+      <c r="E46" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7462,7 +7462,7 @@
       <c r="D47" t="s">
         <v>183</v>
       </c>
-      <c r="E47" s="13" t="b">
+      <c r="E47" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7479,7 +7479,7 @@
       <c r="D48" t="s">
         <v>151</v>
       </c>
-      <c r="E48" s="13" t="b">
+      <c r="E48" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7496,7 +7496,7 @@
       <c r="D49" t="s">
         <v>337</v>
       </c>
-      <c r="E49" s="13" t="b">
+      <c r="E49" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7513,7 +7513,7 @@
       <c r="D50" t="s">
         <v>8</v>
       </c>
-      <c r="E50" s="13" t="b">
+      <c r="E50" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7530,7 +7530,7 @@
       <c r="D51" t="s">
         <v>339</v>
       </c>
-      <c r="E51" s="13" t="b">
+      <c r="E51" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7547,7 +7547,7 @@
       <c r="D52" t="s">
         <v>252</v>
       </c>
-      <c r="E52" s="13" t="b">
+      <c r="E52" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7564,7 +7564,7 @@
       <c r="D53" t="s">
         <v>52</v>
       </c>
-      <c r="E53" s="13" t="b">
+      <c r="E53" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7581,7 +7581,7 @@
       <c r="D54" t="s">
         <v>65</v>
       </c>
-      <c r="E54" s="13" t="b">
+      <c r="E54" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7598,7 +7598,7 @@
       <c r="D55" t="s">
         <v>341</v>
       </c>
-      <c r="E55" s="13" t="b">
+      <c r="E55" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7615,7 +7615,7 @@
       <c r="D56" t="s">
         <v>145</v>
       </c>
-      <c r="E56" s="13" t="b">
+      <c r="E56" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7632,7 +7632,7 @@
       <c r="D57" t="s">
         <v>343</v>
       </c>
-      <c r="E57" s="13" t="b">
+      <c r="E57" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7649,7 +7649,7 @@
       <c r="D58" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="13" t="b">
+      <c r="E58" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7666,7 +7666,7 @@
       <c r="D59" t="s">
         <v>37</v>
       </c>
-      <c r="E59" s="13" t="b">
+      <c r="E59" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7683,7 +7683,7 @@
       <c r="D60" t="s">
         <v>130</v>
       </c>
-      <c r="E60" s="13" t="b">
+      <c r="E60" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7700,7 +7700,7 @@
       <c r="D61" t="s">
         <v>106</v>
       </c>
-      <c r="E61" s="13" t="b">
+      <c r="E61" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7717,7 +7717,7 @@
       <c r="D62" t="s">
         <v>124</v>
       </c>
-      <c r="E62" s="13" t="b">
+      <c r="E62" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7734,7 +7734,7 @@
       <c r="D63" t="s">
         <v>20</v>
       </c>
-      <c r="E63" s="13" t="b">
+      <c r="E63" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7751,7 +7751,7 @@
       <c r="D64" t="s">
         <v>86</v>
       </c>
-      <c r="E64" s="13" t="b">
+      <c r="E64" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7768,7 +7768,7 @@
       <c r="D65" t="s">
         <v>173</v>
       </c>
-      <c r="E65" s="13" t="b">
+      <c r="E65" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7785,7 +7785,7 @@
       <c r="D66" t="s">
         <v>124</v>
       </c>
-      <c r="E66" s="13" t="b">
+      <c r="E66" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7802,7 +7802,7 @@
       <c r="D67" t="s">
         <v>143</v>
       </c>
-      <c r="E67" s="13" t="b">
+      <c r="E67" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7819,7 +7819,7 @@
       <c r="D68" t="s">
         <v>62</v>
       </c>
-      <c r="E68" s="13" t="b">
+      <c r="E68" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7836,7 +7836,7 @@
       <c r="D69" t="s">
         <v>145</v>
       </c>
-      <c r="E69" s="13" t="b">
+      <c r="E69" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7853,7 +7853,7 @@
       <c r="D70" t="s">
         <v>39</v>
       </c>
-      <c r="E70" s="13" t="b">
+      <c r="E70" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7870,7 +7870,7 @@
       <c r="D71" t="s">
         <v>153</v>
       </c>
-      <c r="E71" s="13" t="b">
+      <c r="E71" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7887,7 +7887,7 @@
       <c r="D72" t="s">
         <v>116</v>
       </c>
-      <c r="E72" s="13" t="b">
+      <c r="E72" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7904,7 +7904,7 @@
       <c r="D73" t="s">
         <v>348</v>
       </c>
-      <c r="E73" s="13" t="b">
+      <c r="E73" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7921,7 +7921,7 @@
       <c r="D74" t="s">
         <v>350</v>
       </c>
-      <c r="E74" s="13" t="b">
+      <c r="E74" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7938,7 +7938,7 @@
       <c r="D75" t="s">
         <v>100</v>
       </c>
-      <c r="E75" s="13" t="b">
+      <c r="E75" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7955,7 +7955,7 @@
       <c r="D76" t="s">
         <v>233</v>
       </c>
-      <c r="E76" s="13" t="b">
+      <c r="E76" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7972,7 +7972,7 @@
       <c r="D77" t="s">
         <v>143</v>
       </c>
-      <c r="E77" s="13" t="b">
+      <c r="E77" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7989,7 +7989,7 @@
       <c r="D78" t="s">
         <v>352</v>
       </c>
-      <c r="E78" s="13" t="b">
+      <c r="E78" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8006,7 +8006,7 @@
       <c r="D79" t="s">
         <v>186</v>
       </c>
-      <c r="E79" s="13" t="b">
+      <c r="E79" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8023,7 +8023,7 @@
       <c r="D80" t="s">
         <v>211</v>
       </c>
-      <c r="E80" s="13" t="b">
+      <c r="E80" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8040,7 +8040,7 @@
       <c r="D81" t="s">
         <v>170</v>
       </c>
-      <c r="E81" s="13" t="b">
+      <c r="E81" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8057,7 +8057,7 @@
       <c r="D82" t="s">
         <v>133</v>
       </c>
-      <c r="E82" s="13" t="b">
+      <c r="E82" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8074,7 +8074,7 @@
       <c r="D83" t="s">
         <v>170</v>
       </c>
-      <c r="E83" s="13" t="b">
+      <c r="E83" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8091,7 +8091,7 @@
       <c r="D84" t="s">
         <v>355</v>
       </c>
-      <c r="E84" s="13" t="b">
+      <c r="E84" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8108,7 +8108,7 @@
       <c r="D85" t="s">
         <v>95</v>
       </c>
-      <c r="E85" s="13" t="b">
+      <c r="E85" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8125,7 +8125,7 @@
       <c r="D86" t="s">
         <v>12</v>
       </c>
-      <c r="E86" s="13" t="b">
+      <c r="E86" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8142,7 +8142,7 @@
       <c r="D87" t="s">
         <v>95</v>
       </c>
-      <c r="E87" s="13" t="b">
+      <c r="E87" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8159,7 +8159,7 @@
       <c r="D88" t="s">
         <v>337</v>
       </c>
-      <c r="E88" s="13" t="b">
+      <c r="E88" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8176,7 +8176,7 @@
       <c r="D89" t="s">
         <v>139</v>
       </c>
-      <c r="E89" s="13" t="b">
+      <c r="E89" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8193,7 +8193,7 @@
       <c r="D90" t="s">
         <v>119</v>
       </c>
-      <c r="E90" s="13" t="b">
+      <c r="E90" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8210,7 +8210,7 @@
       <c r="D91" t="s">
         <v>268</v>
       </c>
-      <c r="E91" s="13" t="b">
+      <c r="E91" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8227,7 +8227,7 @@
       <c r="D92" t="s">
         <v>357</v>
       </c>
-      <c r="E92" s="13" t="b">
+      <c r="E92" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8244,7 +8244,7 @@
       <c r="D93" t="s">
         <v>359</v>
       </c>
-      <c r="E93" s="13" t="b">
+      <c r="E93" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8261,7 +8261,7 @@
       <c r="D94" t="s">
         <v>361</v>
       </c>
-      <c r="E94" s="13" t="b">
+      <c r="E94" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8278,7 +8278,7 @@
       <c r="D95" t="s">
         <v>362</v>
       </c>
-      <c r="E95" s="13" t="b">
+      <c r="E95" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8295,7 +8295,7 @@
       <c r="D96" t="s">
         <v>29</v>
       </c>
-      <c r="E96" s="13" t="b">
+      <c r="E96" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8312,7 +8312,7 @@
       <c r="D97" t="s">
         <v>56</v>
       </c>
-      <c r="E97" s="13" t="b">
+      <c r="E97" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8329,7 +8329,7 @@
       <c r="D98" t="s">
         <v>29</v>
       </c>
-      <c r="E98" s="13" t="b">
+      <c r="E98" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8346,7 +8346,7 @@
       <c r="D99" t="s">
         <v>12</v>
       </c>
-      <c r="E99" s="13" t="b">
+      <c r="E99" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8363,7 +8363,7 @@
       <c r="D100" t="s">
         <v>91</v>
       </c>
-      <c r="E100" s="13" t="b">
+      <c r="E100" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8380,7 +8380,7 @@
       <c r="D101" t="s">
         <v>239</v>
       </c>
-      <c r="E101" s="13" t="b">
+      <c r="E101" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8397,7 +8397,7 @@
       <c r="D102" t="s">
         <v>366</v>
       </c>
-      <c r="E102" s="13" t="b">
+      <c r="E102" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8414,7 +8414,7 @@
       <c r="D103" t="s">
         <v>59</v>
       </c>
-      <c r="E103" s="13" t="b">
+      <c r="E103" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8431,7 +8431,7 @@
       <c r="D104" t="s">
         <v>35</v>
       </c>
-      <c r="E104" s="13" t="b">
+      <c r="E104" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8448,7 +8448,7 @@
       <c r="D105" t="s">
         <v>368</v>
       </c>
-      <c r="E105" s="13" t="b">
+      <c r="E105" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8465,7 +8465,7 @@
       <c r="D106" t="s">
         <v>10</v>
       </c>
-      <c r="E106" s="13" t="b">
+      <c r="E106" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8482,7 +8482,7 @@
       <c r="D107" t="s">
         <v>193</v>
       </c>
-      <c r="E107" s="13" t="b">
+      <c r="E107" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8499,7 +8499,7 @@
       <c r="D108" t="s">
         <v>93</v>
       </c>
-      <c r="E108" s="13" t="b">
+      <c r="E108" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8516,7 +8516,7 @@
       <c r="D109" t="s">
         <v>130</v>
       </c>
-      <c r="E109" s="13" t="b">
+      <c r="E109" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8533,7 +8533,7 @@
       <c r="D110" t="s">
         <v>82</v>
       </c>
-      <c r="E110" s="13" t="b">
+      <c r="E110" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8550,7 +8550,7 @@
       <c r="D111" t="s">
         <v>110</v>
       </c>
-      <c r="E111" s="13" t="b">
+      <c r="E111" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8567,7 +8567,7 @@
       <c r="D112" t="s">
         <v>128</v>
       </c>
-      <c r="E112" s="13" t="b">
+      <c r="E112" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8584,7 +8584,7 @@
       <c r="D113" t="s">
         <v>371</v>
       </c>
-      <c r="E113" s="13" t="b">
+      <c r="E113" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8601,7 +8601,7 @@
       <c r="D114" t="s">
         <v>112</v>
       </c>
-      <c r="E114" s="13" t="b">
+      <c r="E114" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8618,7 +8618,7 @@
       <c r="D115" t="s">
         <v>374</v>
       </c>
-      <c r="E115" s="13" t="b">
+      <c r="E115" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8635,7 +8635,7 @@
       <c r="D116" t="s">
         <v>350</v>
       </c>
-      <c r="E116" s="13" t="b">
+      <c r="E116" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8652,7 +8652,7 @@
       <c r="D117" t="s">
         <v>250</v>
       </c>
-      <c r="E117" s="13" t="b">
+      <c r="E117" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8669,7 +8669,7 @@
       <c r="D118" t="s">
         <v>213</v>
       </c>
-      <c r="E118" s="13" t="b">
+      <c r="E118" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8686,7 +8686,7 @@
       <c r="D119" t="s">
         <v>177</v>
       </c>
-      <c r="E119" s="13" t="b">
+      <c r="E119" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8703,7 +8703,7 @@
       <c r="D120" t="s">
         <v>378</v>
       </c>
-      <c r="E120" s="13" t="b">
+      <c r="E120" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8720,7 +8720,7 @@
       <c r="D121" t="s">
         <v>12</v>
       </c>
-      <c r="E121" s="13" t="b">
+      <c r="E121" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8737,7 +8737,7 @@
       <c r="D122" t="s">
         <v>112</v>
       </c>
-      <c r="E122" s="13" t="b">
+      <c r="E122" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8754,7 +8754,7 @@
       <c r="D123" t="s">
         <v>380</v>
       </c>
-      <c r="E123" s="13" t="b">
+      <c r="E123" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8771,7 +8771,7 @@
       <c r="D124" t="s">
         <v>382</v>
       </c>
-      <c r="E124" s="13" t="b">
+      <c r="E124" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8788,7 +8788,7 @@
       <c r="D125" t="s">
         <v>371</v>
       </c>
-      <c r="E125" s="13" t="b">
+      <c r="E125" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8805,7 +8805,7 @@
       <c r="D126" t="s">
         <v>383</v>
       </c>
-      <c r="E126" s="13" t="b">
+      <c r="E126" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8822,7 +8822,7 @@
       <c r="D127" t="s">
         <v>385</v>
       </c>
-      <c r="E127" s="13" t="b">
+      <c r="E127" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8839,7 +8839,7 @@
       <c r="D128" t="s">
         <v>387</v>
       </c>
-      <c r="E128" s="13" t="b">
+      <c r="E128" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8856,7 +8856,7 @@
       <c r="D129" t="s">
         <v>310</v>
       </c>
-      <c r="E129" s="13" t="b">
+      <c r="E129" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8873,7 +8873,7 @@
       <c r="D130" t="s">
         <v>165</v>
       </c>
-      <c r="E130" s="13" t="b">
+      <c r="E130" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8890,7 +8890,7 @@
       <c r="D131" t="s">
         <v>204</v>
       </c>
-      <c r="E131" s="13" t="b">
+      <c r="E131" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8907,7 +8907,7 @@
       <c r="D132" t="s">
         <v>233</v>
       </c>
-      <c r="E132" s="13" t="b">
+      <c r="E132" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8924,7 +8924,7 @@
       <c r="D133" t="s">
         <v>323</v>
       </c>
-      <c r="E133" s="13" t="b">
+      <c r="E133" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8941,7 +8941,7 @@
       <c r="D134" t="s">
         <v>173</v>
       </c>
-      <c r="E134" s="13" t="b">
+      <c r="E134" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8958,7 +8958,7 @@
       <c r="D135" t="s">
         <v>137</v>
       </c>
-      <c r="E135" s="13" t="b">
+      <c r="E135" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8975,7 +8975,7 @@
       <c r="D136" t="s">
         <v>391</v>
       </c>
-      <c r="E136" s="13" t="b">
+      <c r="E136" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -8992,7 +8992,7 @@
       <c r="D137" t="s">
         <v>226</v>
       </c>
-      <c r="E137" s="13" t="b">
+      <c r="E137" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9009,7 +9009,7 @@
       <c r="D138" t="s">
         <v>393</v>
       </c>
-      <c r="E138" s="13" t="b">
+      <c r="E138" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9026,7 +9026,7 @@
       <c r="D139" t="s">
         <v>209</v>
       </c>
-      <c r="E139" s="13" t="b">
+      <c r="E139" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9043,7 +9043,7 @@
       <c r="D140" t="s">
         <v>206</v>
       </c>
-      <c r="E140" s="13" t="b">
+      <c r="E140" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9060,7 +9060,7 @@
       <c r="D141" t="s">
         <v>395</v>
       </c>
-      <c r="E141" s="13" t="b">
+      <c r="E141" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9077,7 +9077,7 @@
       <c r="D142" t="s">
         <v>397</v>
       </c>
-      <c r="E142" s="13" t="b">
+      <c r="E142" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9094,7 +9094,7 @@
       <c r="D143" t="s">
         <v>160</v>
       </c>
-      <c r="E143" s="13" t="b">
+      <c r="E143" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9111,7 +9111,7 @@
       <c r="D144" t="s">
         <v>399</v>
       </c>
-      <c r="E144" s="13" t="b">
+      <c r="E144" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9128,7 +9128,7 @@
       <c r="D145" t="s">
         <v>401</v>
       </c>
-      <c r="E145" s="13" t="b">
+      <c r="E145" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9145,7 +9145,7 @@
       <c r="D146" t="s">
         <v>283</v>
       </c>
-      <c r="E146" s="13" t="b">
+      <c r="E146" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9162,7 +9162,7 @@
       <c r="D147" t="s">
         <v>403</v>
       </c>
-      <c r="E147" s="13" t="b">
+      <c r="E147" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9179,7 +9179,7 @@
       <c r="D148" t="s">
         <v>224</v>
       </c>
-      <c r="E148" s="13" t="b">
+      <c r="E148" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9196,7 +9196,7 @@
       <c r="D149" t="s">
         <v>405</v>
       </c>
-      <c r="E149" s="13" t="b">
+      <c r="E149" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9213,7 +9213,7 @@
       <c r="D150" t="s">
         <v>128</v>
       </c>
-      <c r="E150" s="13" t="b">
+      <c r="E150" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9230,7 +9230,7 @@
       <c r="D151" t="s">
         <v>262</v>
       </c>
-      <c r="E151" s="13" t="b">
+      <c r="E151" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9247,7 +9247,7 @@
       <c r="D152" t="s">
         <v>188</v>
       </c>
-      <c r="E152" s="13" t="b">
+      <c r="E152" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9264,7 +9264,7 @@
       <c r="D153" t="s">
         <v>407</v>
       </c>
-      <c r="E153" s="13" t="b">
+      <c r="E153" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9281,7 +9281,7 @@
       <c r="D154" t="s">
         <v>200</v>
       </c>
-      <c r="E154" s="13" t="b">
+      <c r="E154" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9298,7 +9298,7 @@
       <c r="D155" t="s">
         <v>48</v>
       </c>
-      <c r="E155" s="13" t="b">
+      <c r="E155" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9315,7 +9315,7 @@
       <c r="D156" t="s">
         <v>409</v>
       </c>
-      <c r="E156" s="13" t="b">
+      <c r="E156" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9332,7 +9332,7 @@
       <c r="D157" t="s">
         <v>75</v>
       </c>
-      <c r="E157" s="13" t="b">
+      <c r="E157" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9349,7 +9349,7 @@
       <c r="D158" t="s">
         <v>412</v>
       </c>
-      <c r="E158" s="13" t="b">
+      <c r="E158" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9366,7 +9366,7 @@
       <c r="D159" t="s">
         <v>304</v>
       </c>
-      <c r="E159" s="13" t="b">
+      <c r="E159" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9383,7 +9383,7 @@
       <c r="D160" t="s">
         <v>12</v>
       </c>
-      <c r="E160" s="13" t="b">
+      <c r="E160" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9400,7 +9400,7 @@
       <c r="D161" t="s">
         <v>414</v>
       </c>
-      <c r="E161" s="13" t="b">
+      <c r="E161" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9417,7 +9417,7 @@
       <c r="D162" t="s">
         <v>260</v>
       </c>
-      <c r="E162" s="13" t="b">
+      <c r="E162" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9434,7 +9434,7 @@
       <c r="D163" t="s">
         <v>84</v>
       </c>
-      <c r="E163" s="13" t="b">
+      <c r="E163" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9451,7 +9451,7 @@
       <c r="D164" t="s">
         <v>417</v>
       </c>
-      <c r="E164" s="13" t="b">
+      <c r="E164" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9468,7 +9468,7 @@
       <c r="D165" t="s">
         <v>419</v>
       </c>
-      <c r="E165" s="13" t="b">
+      <c r="E165" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9485,7 +9485,7 @@
       <c r="D166" t="s">
         <v>230</v>
       </c>
-      <c r="E166" s="13" t="b">
+      <c r="E166" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9502,7 +9502,7 @@
       <c r="D167" t="s">
         <v>194</v>
       </c>
-      <c r="E167" s="13" t="b">
+      <c r="E167" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9519,7 +9519,7 @@
       <c r="D168" t="s">
         <v>422</v>
       </c>
-      <c r="E168" s="13" t="b">
+      <c r="E168" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9536,7 +9536,7 @@
       <c r="D169" t="s">
         <v>289</v>
       </c>
-      <c r="E169" s="13" t="b">
+      <c r="E169" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9553,7 +9553,7 @@
       <c r="D170" t="s">
         <v>170</v>
       </c>
-      <c r="E170" s="13" t="b">
+      <c r="E170" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9570,7 +9570,7 @@
       <c r="D171" t="s">
         <v>84</v>
       </c>
-      <c r="E171" s="13" t="b">
+      <c r="E171" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9587,7 +9587,7 @@
       <c r="D172" t="s">
         <v>112</v>
       </c>
-      <c r="E172" s="13" t="b">
+      <c r="E172" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9604,7 +9604,7 @@
       <c r="D173" t="s">
         <v>198</v>
       </c>
-      <c r="E173" s="13" t="b">
+      <c r="E173" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9621,7 +9621,7 @@
       <c r="D174" t="s">
         <v>290</v>
       </c>
-      <c r="E174" s="13" t="b">
+      <c r="E174" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9638,7 +9638,7 @@
       <c r="D175" t="s">
         <v>35</v>
       </c>
-      <c r="E175" s="13" t="b">
+      <c r="E175" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9655,7 +9655,7 @@
       <c r="D176" t="s">
         <v>427</v>
       </c>
-      <c r="E176" s="13" t="b">
+      <c r="E176" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9672,7 +9672,7 @@
       <c r="D177" t="s">
         <v>247</v>
       </c>
-      <c r="E177" s="13" t="b">
+      <c r="E177" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9689,7 +9689,7 @@
       <c r="D178" t="s">
         <v>168</v>
       </c>
-      <c r="E178" s="13" t="b">
+      <c r="E178" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9706,7 +9706,7 @@
       <c r="D179" t="s">
         <v>429</v>
       </c>
-      <c r="E179" s="13" t="b">
+      <c r="E179" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9723,7 +9723,7 @@
       <c r="D180" t="s">
         <v>431</v>
       </c>
-      <c r="E180" s="13" t="b">
+      <c r="E180" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9740,7 +9740,7 @@
       <c r="D181" t="s">
         <v>433</v>
       </c>
-      <c r="E181" s="13" t="b">
+      <c r="E181" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9757,7 +9757,7 @@
       <c r="D182" t="s">
         <v>22</v>
       </c>
-      <c r="E182" s="13" t="b">
+      <c r="E182" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9774,7 +9774,7 @@
       <c r="D183" t="s">
         <v>380</v>
       </c>
-      <c r="E183" s="13" t="b">
+      <c r="E183" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9791,7 +9791,7 @@
       <c r="D184" t="s">
         <v>167</v>
       </c>
-      <c r="E184" s="13" t="b">
+      <c r="E184" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9808,7 +9808,7 @@
       <c r="D185" t="s">
         <v>270</v>
       </c>
-      <c r="E185" s="13" t="b">
+      <c r="E185" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9825,7 +9825,7 @@
       <c r="D186" t="s">
         <v>193</v>
       </c>
-      <c r="E186" s="13" t="b">
+      <c r="E186" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9842,7 +9842,7 @@
       <c r="D187" t="s">
         <v>179</v>
       </c>
-      <c r="E187" s="13" t="b">
+      <c r="E187" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9859,7 +9859,7 @@
       <c r="D188" t="s">
         <v>287</v>
       </c>
-      <c r="E188" s="13" t="b">
+      <c r="E188" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9876,7 +9876,7 @@
       <c r="D189" t="s">
         <v>438</v>
       </c>
-      <c r="E189" s="13" t="b">
+      <c r="E189" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9893,7 +9893,7 @@
       <c r="D190" t="s">
         <v>327</v>
       </c>
-      <c r="E190" s="13" t="b">
+      <c r="E190" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9910,7 +9910,7 @@
       <c r="D191" t="s">
         <v>14</v>
       </c>
-      <c r="E191" s="13" t="b">
+      <c r="E191" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9927,7 +9927,7 @@
       <c r="D192" t="s">
         <v>440</v>
       </c>
-      <c r="E192" s="13" t="b">
+      <c r="E192" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9944,7 +9944,7 @@
       <c r="D193" t="s">
         <v>442</v>
       </c>
-      <c r="E193" s="13" t="b">
+      <c r="E193" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9961,7 +9961,7 @@
       <c r="D194" t="s">
         <v>443</v>
       </c>
-      <c r="E194" s="13" t="b">
+      <c r="E194" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9978,7 +9978,7 @@
       <c r="D195" t="s">
         <v>306</v>
       </c>
-      <c r="E195" s="13" t="b">
+      <c r="E195" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -9995,7 +9995,7 @@
       <c r="D196" t="s">
         <v>445</v>
       </c>
-      <c r="E196" s="13" t="b">
+      <c r="E196" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -10012,7 +10012,7 @@
       <c r="D197" t="s">
         <v>447</v>
       </c>
-      <c r="E197" s="13" t="b">
+      <c r="E197" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -10029,7 +10029,7 @@
       <c r="D198" t="s">
         <v>73</v>
       </c>
-      <c r="E198" s="13" t="b">
+      <c r="E198" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -10046,7 +10046,7 @@
       <c r="D199" t="s">
         <v>298</v>
       </c>
-      <c r="E199" s="13" t="b">
+      <c r="E199" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -10063,7 +10063,7 @@
       <c r="D200" t="s">
         <v>450</v>
       </c>
-      <c r="E200" s="13" t="b">
+      <c r="E200" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -10080,7 +10080,7 @@
       <c r="D201" t="s">
         <v>452</v>
       </c>
-      <c r="E201" s="13" t="b">
+      <c r="E201" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17618,7 +17618,7 @@
       <c r="D35" t="s">
         <v>170</v>
       </c>
-      <c r="E35" s="13" t="b">
+      <c r="E35" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17635,7 +17635,7 @@
       <c r="D36" t="s">
         <v>339</v>
       </c>
-      <c r="E36" s="13" t="b">
+      <c r="E36" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17652,7 +17652,7 @@
       <c r="D37" t="s">
         <v>710</v>
       </c>
-      <c r="E37" s="13" t="b">
+      <c r="E37" s="8" t="b">
         <v>1</v>
       </c>
       <c r="F37" t="s">
@@ -17672,7 +17672,7 @@
       <c r="D38" t="s">
         <v>151</v>
       </c>
-      <c r="E38" s="13" t="b">
+      <c r="E38" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17689,7 +17689,7 @@
       <c r="D39" t="s">
         <v>18</v>
       </c>
-      <c r="E39" s="13" t="b">
+      <c r="E39" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17706,7 +17706,7 @@
       <c r="D40" t="s">
         <v>33</v>
       </c>
-      <c r="E40" s="13" t="b">
+      <c r="E40" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17723,7 +17723,7 @@
       <c r="D41" t="s">
         <v>241</v>
       </c>
-      <c r="E41" s="13" t="b">
+      <c r="E41" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17740,7 +17740,7 @@
       <c r="D42" t="s">
         <v>100</v>
       </c>
-      <c r="E42" s="13" t="b">
+      <c r="E42" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17757,7 +17757,7 @@
       <c r="D43" t="s">
         <v>110</v>
       </c>
-      <c r="E43" s="13" t="b">
+      <c r="E43" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17774,7 +17774,7 @@
       <c r="D44" t="s">
         <v>170</v>
       </c>
-      <c r="E44" s="13" t="b">
+      <c r="E44" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17791,7 +17791,7 @@
       <c r="D45" t="s">
         <v>447</v>
       </c>
-      <c r="E45" s="13" t="b">
+      <c r="E45" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17808,7 +17808,7 @@
       <c r="D46" t="s">
         <v>170</v>
       </c>
-      <c r="E46" s="13" t="b">
+      <c r="E46" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17825,7 +17825,7 @@
       <c r="D47" t="s">
         <v>519</v>
       </c>
-      <c r="E47" s="13" t="b">
+      <c r="E47" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17842,7 +17842,7 @@
       <c r="D48" t="s">
         <v>29</v>
       </c>
-      <c r="E48" s="13" t="b">
+      <c r="E48" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17859,7 +17859,7 @@
       <c r="D49" t="s">
         <v>460</v>
       </c>
-      <c r="E49" s="13" t="b">
+      <c r="E49" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17876,7 +17876,7 @@
       <c r="D50" t="s">
         <v>462</v>
       </c>
-      <c r="E50" s="13" t="b">
+      <c r="E50" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17893,7 +17893,7 @@
       <c r="D51" t="s">
         <v>124</v>
       </c>
-      <c r="E51" s="13" t="b">
+      <c r="E51" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17910,7 +17910,7 @@
       <c r="D52" t="s">
         <v>371</v>
       </c>
-      <c r="E52" s="13" t="b">
+      <c r="E52" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17927,7 +17927,7 @@
       <c r="D53" t="s">
         <v>686</v>
       </c>
-      <c r="E53" s="13" t="b">
+      <c r="E53" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17944,7 +17944,7 @@
       <c r="D54" t="s">
         <v>170</v>
       </c>
-      <c r="E54" s="13" t="b">
+      <c r="E54" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17961,7 +17961,7 @@
       <c r="D55" t="s">
         <v>239</v>
       </c>
-      <c r="E55" s="13" t="b">
+      <c r="E55" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17978,7 +17978,7 @@
       <c r="D56" t="s">
         <v>457</v>
       </c>
-      <c r="E56" s="13" t="b">
+      <c r="E56" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -17995,7 +17995,7 @@
       <c r="D57" t="s">
         <v>442</v>
       </c>
-      <c r="E57" s="13" t="b">
+      <c r="E57" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18012,7 +18012,7 @@
       <c r="D58" t="s">
         <v>56</v>
       </c>
-      <c r="E58" s="13" t="b">
+      <c r="E58" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18029,7 +18029,7 @@
       <c r="D59" t="s">
         <v>137</v>
       </c>
-      <c r="E59" s="13" t="b">
+      <c r="E59" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18046,7 +18046,7 @@
       <c r="D60" t="s">
         <v>419</v>
       </c>
-      <c r="E60" s="13" t="b">
+      <c r="E60" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18063,7 +18063,7 @@
       <c r="D61" t="s">
         <v>95</v>
       </c>
-      <c r="E61" s="13" t="b">
+      <c r="E61" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18080,7 +18080,7 @@
       <c r="D62" t="s">
         <v>158</v>
       </c>
-      <c r="E62" s="13" t="b">
+      <c r="E62" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18097,7 +18097,7 @@
       <c r="D63" t="s">
         <v>155</v>
       </c>
-      <c r="E63" s="13" t="b">
+      <c r="E63" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18114,7 +18114,7 @@
       <c r="D64" t="s">
         <v>12</v>
       </c>
-      <c r="E64" s="13" t="b">
+      <c r="E64" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18131,7 +18131,7 @@
       <c r="D65" t="s">
         <v>73</v>
       </c>
-      <c r="E65" s="13" t="b">
+      <c r="E65" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18148,7 +18148,7 @@
       <c r="D66" t="s">
         <v>170</v>
       </c>
-      <c r="E66" s="13" t="b">
+      <c r="E66" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18165,7 +18165,7 @@
       <c r="D67" t="s">
         <v>720</v>
       </c>
-      <c r="E67" s="13" t="b">
+      <c r="E67" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18182,7 +18182,7 @@
       <c r="D68" t="s">
         <v>100</v>
       </c>
-      <c r="E68" s="13" t="b">
+      <c r="E68" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18199,7 +18199,7 @@
       <c r="D69" t="s">
         <v>31</v>
       </c>
-      <c r="E69" s="13" t="b">
+      <c r="E69" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18216,7 +18216,7 @@
       <c r="D70" t="s">
         <v>170</v>
       </c>
-      <c r="E70" s="13" t="b">
+      <c r="E70" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18233,7 +18233,7 @@
       <c r="D71" t="s">
         <v>527</v>
       </c>
-      <c r="E71" s="13" t="b">
+      <c r="E71" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18250,7 +18250,7 @@
       <c r="D72" t="s">
         <v>523</v>
       </c>
-      <c r="E72" s="13" t="b">
+      <c r="E72" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18267,7 +18267,7 @@
       <c r="D73" t="s">
         <v>516</v>
       </c>
-      <c r="E73" s="13" t="b">
+      <c r="E73" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18284,7 +18284,7 @@
       <c r="D74" t="s">
         <v>106</v>
       </c>
-      <c r="E74" s="13" t="b">
+      <c r="E74" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18301,7 +18301,7 @@
       <c r="D75" t="s">
         <v>262</v>
       </c>
-      <c r="E75" s="13" t="b">
+      <c r="E75" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18318,7 +18318,7 @@
       <c r="D76" t="s">
         <v>84</v>
       </c>
-      <c r="E76" s="13" t="b">
+      <c r="E76" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18335,7 +18335,7 @@
       <c r="D77" t="s">
         <v>84</v>
       </c>
-      <c r="E77" s="13" t="b">
+      <c r="E77" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18352,7 +18352,7 @@
       <c r="D78" t="s">
         <v>726</v>
       </c>
-      <c r="E78" s="13" t="b">
+      <c r="E78" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18369,7 +18369,7 @@
       <c r="D79" t="s">
         <v>139</v>
       </c>
-      <c r="E79" s="13" t="b">
+      <c r="E79" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18386,7 +18386,7 @@
       <c r="D80" t="s">
         <v>158</v>
       </c>
-      <c r="E80" s="13" t="b">
+      <c r="E80" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18403,7 +18403,7 @@
       <c r="D81" t="s">
         <v>130</v>
       </c>
-      <c r="E81" s="13" t="b">
+      <c r="E81" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18420,7 +18420,7 @@
       <c r="D82" t="s">
         <v>596</v>
       </c>
-      <c r="E82" s="13" t="b">
+      <c r="E82" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18437,7 +18437,7 @@
       <c r="D83" t="s">
         <v>729</v>
       </c>
-      <c r="E83" s="13" t="b">
+      <c r="E83" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18454,7 +18454,7 @@
       <c r="D84" t="s">
         <v>684</v>
       </c>
-      <c r="E84" s="13" t="b">
+      <c r="E84" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18471,7 +18471,7 @@
       <c r="D85" t="s">
         <v>357</v>
       </c>
-      <c r="E85" s="13" t="b">
+      <c r="E85" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18488,7 +18488,7 @@
       <c r="D86" t="s">
         <v>414</v>
       </c>
-      <c r="E86" s="13" t="b">
+      <c r="E86" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18505,7 +18505,7 @@
       <c r="D87" t="s">
         <v>12</v>
       </c>
-      <c r="E87" s="13" t="b">
+      <c r="E87" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18522,7 +18522,7 @@
       <c r="D88" t="s">
         <v>734</v>
       </c>
-      <c r="E88" s="13" t="b">
+      <c r="E88" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18539,7 +18539,7 @@
       <c r="D89" t="s">
         <v>160</v>
       </c>
-      <c r="E89" s="13" t="b">
+      <c r="E89" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18556,7 +18556,7 @@
       <c r="D90" t="s">
         <v>228</v>
       </c>
-      <c r="E90" s="13" t="b">
+      <c r="E90" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18573,7 +18573,7 @@
       <c r="D91" t="s">
         <v>320</v>
       </c>
-      <c r="E91" s="13" t="b">
+      <c r="E91" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18590,7 +18590,7 @@
       <c r="D92" t="s">
         <v>738</v>
       </c>
-      <c r="E92" s="13" t="b">
+      <c r="E92" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18607,7 +18607,7 @@
       <c r="D93" t="s">
         <v>116</v>
       </c>
-      <c r="E93" s="13" t="b">
+      <c r="E93" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18624,7 +18624,7 @@
       <c r="D94" t="s">
         <v>740</v>
       </c>
-      <c r="E94" s="13" t="b">
+      <c r="E94" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18641,7 +18641,7 @@
       <c r="D95" t="s">
         <v>742</v>
       </c>
-      <c r="E95" s="13" t="b">
+      <c r="E95" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18658,7 +18658,7 @@
       <c r="D96" t="s">
         <v>168</v>
       </c>
-      <c r="E96" s="13" t="b">
+      <c r="E96" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18675,7 +18675,7 @@
       <c r="D97" t="s">
         <v>442</v>
       </c>
-      <c r="E97" s="13" t="b">
+      <c r="E97" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18692,7 +18692,7 @@
       <c r="D98" t="s">
         <v>151</v>
       </c>
-      <c r="E98" s="13" t="b">
+      <c r="E98" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18709,7 +18709,7 @@
       <c r="D99" t="s">
         <v>304</v>
       </c>
-      <c r="E99" s="13" t="b">
+      <c r="E99" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18726,7 +18726,7 @@
       <c r="D100" t="s">
         <v>306</v>
       </c>
-      <c r="E100" s="13" t="b">
+      <c r="E100" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18743,7 +18743,7 @@
       <c r="D101" t="s">
         <v>350</v>
       </c>
-      <c r="E101" s="13" t="b">
+      <c r="E101" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18760,7 +18760,7 @@
       <c r="D102" t="s">
         <v>10</v>
       </c>
-      <c r="E102" s="13" t="b">
+      <c r="E102" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18777,7 +18777,7 @@
       <c r="D103" t="s">
         <v>204</v>
       </c>
-      <c r="E103" s="13" t="b">
+      <c r="E103" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18794,7 +18794,7 @@
       <c r="D104" t="s">
         <v>310</v>
       </c>
-      <c r="E104" s="13" t="b">
+      <c r="E104" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18811,7 +18811,7 @@
       <c r="D105" t="s">
         <v>170</v>
       </c>
-      <c r="E105" s="13" t="b">
+      <c r="E105" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18828,7 +18828,7 @@
       <c r="D106" t="s">
         <v>12</v>
       </c>
-      <c r="E106" s="13" t="b">
+      <c r="E106" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18845,7 +18845,7 @@
       <c r="D107" t="s">
         <v>355</v>
       </c>
-      <c r="E107" s="13" t="b">
+      <c r="E107" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18862,7 +18862,7 @@
       <c r="D108" t="s">
         <v>323</v>
       </c>
-      <c r="E108" s="13" t="b">
+      <c r="E108" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18879,7 +18879,7 @@
       <c r="D109" t="s">
         <v>748</v>
       </c>
-      <c r="E109" s="13" t="b">
+      <c r="E109" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18896,7 +18896,7 @@
       <c r="D110" t="s">
         <v>16</v>
       </c>
-      <c r="E110" s="13" t="b">
+      <c r="E110" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18913,7 +18913,7 @@
       <c r="D111" t="s">
         <v>100</v>
       </c>
-      <c r="E111" s="13" t="b">
+      <c r="E111" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18930,7 +18930,7 @@
       <c r="D112" t="s">
         <v>751</v>
       </c>
-      <c r="E112" s="13" t="b">
+      <c r="E112" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18947,7 +18947,7 @@
       <c r="D113" t="s">
         <v>753</v>
       </c>
-      <c r="E113" s="13" t="b">
+      <c r="E113" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18964,7 +18964,7 @@
       <c r="D114" t="s">
         <v>193</v>
       </c>
-      <c r="E114" s="13" t="b">
+      <c r="E114" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18981,7 +18981,7 @@
       <c r="D115" t="s">
         <v>755</v>
       </c>
-      <c r="E115" s="13" t="b">
+      <c r="E115" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -18998,7 +18998,7 @@
       <c r="D116" t="s">
         <v>757</v>
       </c>
-      <c r="E116" s="13" t="b">
+      <c r="E116" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19015,7 +19015,7 @@
       <c r="D117" t="s">
         <v>133</v>
       </c>
-      <c r="E117" s="13" t="b">
+      <c r="E117" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19032,7 +19032,7 @@
       <c r="D118" t="s">
         <v>337</v>
       </c>
-      <c r="E118" s="13" t="b">
+      <c r="E118" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19049,7 +19049,7 @@
       <c r="D119" t="s">
         <v>460</v>
       </c>
-      <c r="E119" s="13" t="b">
+      <c r="E119" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19066,7 +19066,7 @@
       <c r="D120" t="s">
         <v>206</v>
       </c>
-      <c r="E120" s="13" t="b">
+      <c r="E120" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19083,7 +19083,7 @@
       <c r="D121" t="s">
         <v>570</v>
       </c>
-      <c r="E121" s="13" t="b">
+      <c r="E121" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19100,7 +19100,7 @@
       <c r="D122" t="s">
         <v>762</v>
       </c>
-      <c r="E122" s="13" t="b">
+      <c r="E122" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19117,7 +19117,7 @@
       <c r="D123" t="s">
         <v>764</v>
       </c>
-      <c r="E123" s="13" t="b">
+      <c r="E123" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19134,7 +19134,7 @@
       <c r="D124" t="s">
         <v>419</v>
       </c>
-      <c r="E124" s="13" t="b">
+      <c r="E124" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19151,7 +19151,7 @@
       <c r="D125" t="s">
         <v>766</v>
       </c>
-      <c r="E125" s="13" t="b">
+      <c r="E125" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19168,7 +19168,7 @@
       <c r="D126" t="s">
         <v>170</v>
       </c>
-      <c r="E126" s="13" t="b">
+      <c r="E126" s="8" t="b">
         <v>0</v>
       </c>
       <c r="F126" t="s">
@@ -19188,7 +19188,7 @@
       <c r="D127" t="s">
         <v>128</v>
       </c>
-      <c r="E127" s="13" t="b">
+      <c r="E127" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19205,7 +19205,7 @@
       <c r="D128" t="s">
         <v>206</v>
       </c>
-      <c r="E128" s="13" t="b">
+      <c r="E128" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19222,7 +19222,7 @@
       <c r="D129" t="s">
         <v>769</v>
       </c>
-      <c r="E129" s="13" t="b">
+      <c r="E129" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19239,7 +19239,7 @@
       <c r="D130" t="s">
         <v>341</v>
       </c>
-      <c r="E130" s="13" t="b">
+      <c r="E130" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19256,7 +19256,7 @@
       <c r="D131" t="s">
         <v>772</v>
       </c>
-      <c r="E131" s="13" t="b">
+      <c r="E131" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19273,7 +19273,7 @@
       <c r="D132" t="s">
         <v>412</v>
       </c>
-      <c r="E132" s="13" t="b">
+      <c r="E132" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19290,7 +19290,7 @@
       <c r="D133" t="s">
         <v>403</v>
       </c>
-      <c r="E133" s="13" t="b">
+      <c r="E133" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19307,7 +19307,7 @@
       <c r="D134" t="s">
         <v>86</v>
       </c>
-      <c r="E134" s="13" t="b">
+      <c r="E134" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19324,7 +19324,7 @@
       <c r="D135" t="s">
         <v>774</v>
       </c>
-      <c r="E135" s="13" t="b">
+      <c r="E135" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19341,7 +19341,7 @@
       <c r="D136" t="s">
         <v>46</v>
       </c>
-      <c r="E136" s="13" t="b">
+      <c r="E136" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19358,7 +19358,7 @@
       <c r="D137" t="s">
         <v>188</v>
       </c>
-      <c r="E137" s="13" t="b">
+      <c r="E137" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19375,7 +19375,7 @@
       <c r="D138" t="s">
         <v>776</v>
       </c>
-      <c r="E138" s="13" t="b">
+      <c r="E138" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19392,7 +19392,7 @@
       <c r="D139" t="s">
         <v>143</v>
       </c>
-      <c r="E139" s="13" t="b">
+      <c r="E139" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19409,7 +19409,7 @@
       <c r="D140" t="s">
         <v>778</v>
       </c>
-      <c r="E140" s="13" t="b">
+      <c r="E140" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19426,7 +19426,7 @@
       <c r="D141" t="s">
         <v>194</v>
       </c>
-      <c r="E141" s="13" t="b">
+      <c r="E141" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19443,7 +19443,7 @@
       <c r="D142" t="s">
         <v>143</v>
       </c>
-      <c r="E142" s="13" t="b">
+      <c r="E142" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19460,7 +19460,7 @@
       <c r="D143" t="s">
         <v>247</v>
       </c>
-      <c r="E143" s="13" t="b">
+      <c r="E143" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19477,7 +19477,7 @@
       <c r="D144" t="s">
         <v>247</v>
       </c>
-      <c r="E144" s="13" t="b">
+      <c r="E144" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19494,7 +19494,7 @@
       <c r="D145" t="s">
         <v>405</v>
       </c>
-      <c r="E145" s="13" t="b">
+      <c r="E145" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19511,7 +19511,7 @@
       <c r="D146" t="s">
         <v>535</v>
       </c>
-      <c r="E146" s="13" t="b">
+      <c r="E146" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19528,7 +19528,7 @@
       <c r="D147" t="s">
         <v>224</v>
       </c>
-      <c r="E147" s="13" t="b">
+      <c r="E147" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19545,7 +19545,7 @@
       <c r="D148" t="s">
         <v>634</v>
       </c>
-      <c r="E148" s="13" t="b">
+      <c r="E148" s="8" t="b">
         <v>0</v>
       </c>
       <c r="F148" t="s">
@@ -19565,7 +19565,7 @@
       <c r="D149" t="s">
         <v>160</v>
       </c>
-      <c r="E149" s="13" t="b">
+      <c r="E149" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19582,7 +19582,7 @@
       <c r="D150" t="s">
         <v>143</v>
       </c>
-      <c r="E150" s="13" t="b">
+      <c r="E150" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19599,7 +19599,7 @@
       <c r="D151" t="s">
         <v>625</v>
       </c>
-      <c r="E151" s="13" t="b">
+      <c r="E151" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19616,7 +19616,7 @@
       <c r="D152" t="s">
         <v>341</v>
       </c>
-      <c r="E152" s="13" t="b">
+      <c r="E152" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19633,7 +19633,7 @@
       <c r="D153" t="s">
         <v>350</v>
       </c>
-      <c r="E153" s="13" t="b">
+      <c r="E153" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19650,7 +19650,7 @@
       <c r="D154" t="s">
         <v>306</v>
       </c>
-      <c r="E154" s="13" t="b">
+      <c r="E154" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19667,7 +19667,7 @@
       <c r="D155" t="s">
         <v>29</v>
       </c>
-      <c r="E155" s="13" t="b">
+      <c r="E155" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19684,7 +19684,7 @@
       <c r="D156" t="s">
         <v>65</v>
       </c>
-      <c r="E156" s="13" t="b">
+      <c r="E156" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19701,7 +19701,7 @@
       <c r="D157" t="s">
         <v>789</v>
       </c>
-      <c r="E157" s="13" t="b">
+      <c r="E157" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19718,7 +19718,7 @@
       <c r="D158" t="s">
         <v>339</v>
       </c>
-      <c r="E158" s="13" t="b">
+      <c r="E158" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19735,7 +19735,7 @@
       <c r="D159" t="s">
         <v>792</v>
       </c>
-      <c r="E159" s="13" t="b">
+      <c r="E159" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19752,7 +19752,7 @@
       <c r="D160" t="s">
         <v>350</v>
       </c>
-      <c r="E160" s="13" t="b">
+      <c r="E160" s="8" t="b">
         <v>0</v>
       </c>
       <c r="F160" t="s">
@@ -19772,7 +19772,7 @@
       <c r="D161" t="s">
         <v>660</v>
       </c>
-      <c r="E161" s="13" t="b">
+      <c r="E161" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19789,7 +19789,7 @@
       <c r="D162" t="s">
         <v>316</v>
       </c>
-      <c r="E162" s="13" t="b">
+      <c r="E162" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19806,7 +19806,7 @@
       <c r="D163" t="s">
         <v>632</v>
       </c>
-      <c r="E163" s="13" t="b">
+      <c r="E163" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19823,7 +19823,7 @@
       <c r="D164" t="s">
         <v>797</v>
       </c>
-      <c r="E164" s="13" t="b">
+      <c r="E164" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19840,7 +19840,7 @@
       <c r="D165" t="s">
         <v>361</v>
       </c>
-      <c r="E165" s="13" t="b">
+      <c r="E165" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19857,7 +19857,7 @@
       <c r="D166" t="s">
         <v>290</v>
       </c>
-      <c r="E166" s="13" t="b">
+      <c r="E166" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19874,7 +19874,7 @@
       <c r="D167" t="s">
         <v>350</v>
       </c>
-      <c r="E167" s="13" t="b">
+      <c r="E167" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19891,7 +19891,7 @@
       <c r="D168" t="s">
         <v>801</v>
       </c>
-      <c r="E168" s="13" t="b">
+      <c r="E168" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19908,7 +19908,7 @@
       <c r="D169" t="s">
         <v>84</v>
       </c>
-      <c r="E169" s="13" t="b">
+      <c r="E169" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19925,7 +19925,7 @@
       <c r="D170" t="s">
         <v>177</v>
       </c>
-      <c r="E170" s="13" t="b">
+      <c r="E170" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19942,7 +19942,7 @@
       <c r="D171" t="s">
         <v>573</v>
       </c>
-      <c r="E171" s="13" t="b">
+      <c r="E171" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19959,7 +19959,7 @@
       <c r="D172" t="s">
         <v>337</v>
       </c>
-      <c r="E172" s="13" t="b">
+      <c r="E172" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19976,7 +19976,7 @@
       <c r="D173" t="s">
         <v>804</v>
       </c>
-      <c r="E173" s="13" t="b">
+      <c r="E173" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -19993,7 +19993,7 @@
       <c r="D174" t="s">
         <v>228</v>
       </c>
-      <c r="E174" s="13" t="b">
+      <c r="E174" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20010,7 +20010,7 @@
       <c r="D175" t="s">
         <v>807</v>
       </c>
-      <c r="E175" s="13" t="b">
+      <c r="E175" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20027,7 +20027,7 @@
       <c r="D176" t="s">
         <v>170</v>
       </c>
-      <c r="E176" s="13" t="b">
+      <c r="E176" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20044,7 +20044,7 @@
       <c r="D177" t="s">
         <v>268</v>
       </c>
-      <c r="E177" s="13" t="b">
+      <c r="E177" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20061,7 +20061,7 @@
       <c r="D178" t="s">
         <v>811</v>
       </c>
-      <c r="E178" s="13" t="b">
+      <c r="E178" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20078,7 +20078,7 @@
       <c r="D179" t="s">
         <v>320</v>
       </c>
-      <c r="E179" s="13" t="b">
+      <c r="E179" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20095,7 +20095,7 @@
       <c r="D180" t="s">
         <v>663</v>
       </c>
-      <c r="E180" s="13" t="b">
+      <c r="E180" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20112,7 +20112,7 @@
       <c r="D181" t="s">
         <v>241</v>
       </c>
-      <c r="E181" s="13" t="b">
+      <c r="E181" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20129,7 +20129,7 @@
       <c r="D182" t="s">
         <v>95</v>
       </c>
-      <c r="E182" s="13" t="b">
+      <c r="E182" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20146,7 +20146,7 @@
       <c r="D183" t="s">
         <v>814</v>
       </c>
-      <c r="E183" s="13" t="b">
+      <c r="E183" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20163,7 +20163,7 @@
       <c r="D184" t="s">
         <v>165</v>
       </c>
-      <c r="E184" s="13" t="b">
+      <c r="E184" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20180,7 +20180,7 @@
       <c r="D185" t="s">
         <v>816</v>
       </c>
-      <c r="E185" s="13" t="b">
+      <c r="E185" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20197,7 +20197,7 @@
       <c r="D186" t="s">
         <v>818</v>
       </c>
-      <c r="E186" s="13" t="b">
+      <c r="E186" s="8" t="b">
         <v>0</v>
       </c>
       <c r="F186" t="s">
@@ -20217,7 +20217,7 @@
       <c r="D187" t="s">
         <v>820</v>
       </c>
-      <c r="E187" s="13" t="b">
+      <c r="E187" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20234,7 +20234,7 @@
       <c r="D188" t="s">
         <v>822</v>
       </c>
-      <c r="E188" s="13" t="b">
+      <c r="E188" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20251,7 +20251,7 @@
       <c r="D189" t="s">
         <v>824</v>
       </c>
-      <c r="E189" s="13" t="b">
+      <c r="E189" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20268,7 +20268,7 @@
       <c r="D190" t="s">
         <v>826</v>
       </c>
-      <c r="E190" s="13" t="b">
+      <c r="E190" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20285,7 +20285,7 @@
       <c r="D191" t="s">
         <v>296</v>
       </c>
-      <c r="E191" s="13" t="b">
+      <c r="E191" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20302,7 +20302,7 @@
       <c r="D192" t="s">
         <v>350</v>
       </c>
-      <c r="E192" s="13" t="b">
+      <c r="E192" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20319,7 +20319,7 @@
       <c r="D193" t="s">
         <v>350</v>
       </c>
-      <c r="E193" s="13" t="b">
+      <c r="E193" s="8" t="b">
         <v>0</v>
       </c>
       <c r="F193" t="s">
@@ -20339,7 +20339,7 @@
       <c r="D194" t="s">
         <v>830</v>
       </c>
-      <c r="E194" s="13" t="b">
+      <c r="E194" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20356,7 +20356,7 @@
       <c r="D195" t="s">
         <v>350</v>
       </c>
-      <c r="E195" s="13" t="b">
+      <c r="E195" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20373,7 +20373,7 @@
       <c r="D196" t="s">
         <v>124</v>
       </c>
-      <c r="E196" s="13" t="b">
+      <c r="E196" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20390,7 +20390,7 @@
       <c r="D197" t="s">
         <v>834</v>
       </c>
-      <c r="E197" s="13" t="b">
+      <c r="E197" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20407,7 +20407,7 @@
       <c r="D198" t="s">
         <v>523</v>
       </c>
-      <c r="E198" s="13" t="b">
+      <c r="E198" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20424,7 +20424,7 @@
       <c r="D199" t="s">
         <v>634</v>
       </c>
-      <c r="E199" s="13" t="b">
+      <c r="E199" s="8" t="b">
         <v>0</v>
       </c>
       <c r="F199" t="s">
@@ -20444,7 +20444,7 @@
       <c r="D200" t="s">
         <v>837</v>
       </c>
-      <c r="E200" s="13" t="b">
+      <c r="E200" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20461,7 +20461,7 @@
       <c r="D201" t="s">
         <v>839</v>
       </c>
-      <c r="E201" s="13" t="b">
+      <c r="E201" s="8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -20555,7 +20555,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>The Weeknd</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="9" t="s">
         <v>842</v>
       </c>
     </row>
@@ -20575,7 +20575,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>Ed Sheeran</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -20593,7 +20593,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>Drake</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -20611,7 +20611,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>Soundtrack</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
@@ -20629,7 +20629,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>Post Malone</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
@@ -20647,7 +20647,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>Migos</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:6" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -20665,7 +20665,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>Original Broadway Cast</v>
       </c>
-      <c r="F10" s="9"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
@@ -20683,7 +20683,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>J. Cole</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="11" t="s">
         <v>843</v>
       </c>
     </row>
@@ -20703,7 +20703,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>Soundtrack</v>
       </c>
-      <c r="F12" s="11"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -20721,7 +20721,7 @@
         <f t="shared" ca="1" si="2"/>
         <v>Metallica</v>
       </c>
-      <c r="F13" s="12"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="5">

</xml_diff>

<commit_message>
Created all album tracks notebook and table
Created notebook and dataframe for all album tracks, exported to csv
</commit_message>
<xml_diff>
--- a/Master Chart Data.xlsx
+++ b/Master Chart Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherineravenwood/Documents/GitHub/Spotify-Five-Year-Analysis-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8658B99F-4E11-F44C-A458-7C35296B201A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633281B1-AB4F-B245-BD50-56A1C9CD8CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{BA16DD78-4E07-0B46-959B-144C800F05BB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{BA16DD78-4E07-0B46-959B-144C800F05BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Top Albums Playlists" sheetId="1" r:id="rId1"/>
@@ -3183,7 +3183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{297D2F08-F1C7-A048-8D03-2A43416905E3}">
   <dimension ref="A1:I201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
+    <sheetView zoomScale="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
@@ -13546,8 +13546,8 @@
   <dimension ref="A1:J201"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="159" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E176" sqref="E176:E201"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F139" sqref="F139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17001,9 +17001,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{281BF527-939F-0B4A-99C4-7919A035DBB5}">
   <dimension ref="A1:J201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B193" sqref="B193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>